<commit_message>
Modified the filters in some tables
</commit_message>
<xml_diff>
--- a/public/sample/addmember.xlsx
+++ b/public/sample/addmember.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="990" yWindow="0" windowWidth="19500" windowHeight="8340"/>
+    <workbookView xWindow="1980" yWindow="0" windowWidth="19500" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -38,9 +35,6 @@
     <t>member_type</t>
   </si>
   <si>
-    <t>email address</t>
-  </si>
-  <si>
     <t>mobile</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>previous church</t>
   </si>
   <si>
-    <t>member_image</t>
-  </si>
-  <si>
     <t>Jeremiah</t>
   </si>
   <si>
@@ -102,6 +93,9 @@
   </si>
   <si>
     <t>Lighthouse Chapel International</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -465,29 +459,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" customWidth="1"/>
-    <col min="14" max="14" width="29.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,92 +488,83 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D2">
+        <v>2045877963</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2">
+        <v>36238</v>
+      </c>
+      <c r="L2" s="2">
+        <v>43794</v>
+      </c>
+      <c r="M2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2">
-        <v>2045877963</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="2">
-        <v>36445</v>
-      </c>
-      <c r="M2" s="2">
-        <v>43750</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix mass upload of members
</commit_message>
<xml_diff>
--- a/public/sample/addmember.xlsx
+++ b/public/sample/addmember.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="0" windowWidth="19500" windowHeight="8340"/>
+    <workbookView xWindow="3960" yWindow="0" windowWidth="19500" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>department</t>
   </si>
   <si>
-    <t>date of birth</t>
-  </si>
-  <si>
     <t>date joined</t>
   </si>
   <si>
@@ -68,34 +65,37 @@
     <t>Jeremiah</t>
   </si>
   <si>
-    <t>Child</t>
-  </si>
-  <si>
     <t>jerry@gmail.com</t>
   </si>
   <si>
-    <t>Ivorian</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Student</t>
-  </si>
-  <si>
     <t>Dansoman A 60</t>
   </si>
   <si>
     <t>Member</t>
   </si>
   <si>
-    <t>Children</t>
-  </si>
-  <si>
     <t>Lighthouse Chapel International</t>
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>bday</t>
+  </si>
+  <si>
+    <t>Ghanaian</t>
+  </si>
+  <si>
+    <t>Business Manager</t>
+  </si>
+  <si>
+    <t>Choir</t>
+  </si>
+  <si>
+    <t>Adult</t>
   </si>
 </sst>
 </file>
@@ -140,10 +140,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,23 +462,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="8" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -485,25 +484,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -518,53 +517,53 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="3">
+        <v>245877963</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2">
+        <v>35348</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2">
-        <v>2045877963</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="2">
+        <v>43748</v>
+      </c>
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="2">
-        <v>36238</v>
-      </c>
-      <c r="L2" s="2">
-        <v>43794</v>
-      </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>